<commit_message>
done w naive mhla
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_6AIML\meh\LLMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587D024F-8EF7-4C4D-970F-69F00A137077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCC0BEF-222E-4B90-8790-D68876F67E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{299E19B8-F4A1-4D4E-BEC0-D6AB4483F225}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Attention</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>model size</t>
+  </si>
+  <si>
+    <t>Flash MHLA</t>
   </si>
 </sst>
 </file>
@@ -487,14 +490,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED386B1-C0DC-41EF-8CB2-758929BC0C80}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5546875" customWidth="1"/>
@@ -670,7 +674,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="2">
-        <v>17463296</v>
+        <v>16939008</v>
       </c>
       <c r="H5">
         <v>8</v>
@@ -811,6 +815,41 @@
         <v>2500</v>
       </c>
       <c r="N8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>256</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>1024</v>
+      </c>
+      <c r="J9" s="1">
+        <v>20000000000000</v>
+      </c>
+      <c r="K9">
+        <v>2500</v>
+      </c>
+      <c r="N9">
         <v>5000</v>
       </c>
     </row>

</xml_diff>